<commit_message>
update to master thesis
</commit_message>
<xml_diff>
--- a/geo_matrix.xlsx
+++ b/geo_matrix.xlsx
@@ -1509,7 +1509,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE64C918-0DDE-4FD0-BB50-DDB8A5AD4ACB}">
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:K60"/>
   <sheetViews>
     <sheetView tabSelected="true" topLeftCell="A15" workbookViewId="0">
       <selection activeCell="M28" sqref="M28"/>
@@ -1517,13 +1517,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.37890625" customWidth="true"/>
+    <col min="1" max="1" width="15.7109375" customWidth="true"/>
     <col min="2" max="2" width="14.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" x14ac:dyDescent="0.3">
       <c r="A1" s="0">
-        <v>0.047975019947768711</v>
+        <v>0.027600000000000003</v>
       </c>
       <c r="B1" s="0">
         <v>0</v>
@@ -1531,18 +1531,18 @@
     </row>
     <row r="2" x14ac:dyDescent="0.3">
       <c r="A2" s="0">
-        <v>0.049717305278328024</v>
+        <v>0.028601294327848414</v>
       </c>
       <c r="B2" s="0">
-        <v>0.0032004970687439429</v>
+        <v>0.0018573501969297143</v>
       </c>
     </row>
     <row r="3" x14ac:dyDescent="0.3">
       <c r="A3" s="0">
-        <v>0.051239006062588882</v>
+        <v>0.029470353337400279</v>
       </c>
       <c r="B3" s="0">
-        <v>0.0066240806869784213</v>
+        <v>0.0038677611022306132</v>
       </c>
       <c r="D3">
         <v>61.984699999999997</v>
@@ -1553,82 +1553,82 @@
     </row>
     <row r="4" x14ac:dyDescent="0.3">
       <c r="A4" s="0">
-        <v>0.052516758968336387</v>
+        <v>0.030188157241896781</v>
       </c>
       <c r="B4" s="0">
-        <v>0.010265196114191962</v>
+        <v>0.0060305643780009096</v>
       </c>
     </row>
     <row r="5" x14ac:dyDescent="0.3">
       <c r="A5" s="0">
-        <v>0.05352489802741877</v>
+        <v>0.030733835508605832</v>
       </c>
       <c r="B5" s="0">
-        <v>0.014119101476175755</v>
+        <v>0.0083431930172362008</v>
       </c>
     </row>
     <row r="6" x14ac:dyDescent="0.3">
       <c r="A6" s="0">
-        <v>0.054233872304327337</v>
+        <v>0.031087106735310802</v>
       </c>
       <c r="B6" s="0">
-        <v>0.018183503972678865</v>
+        <v>0.01079388752235012</v>
       </c>
     </row>
     <row r="7" x14ac:dyDescent="0.3">
       <c r="A7" s="0">
-        <v>0.054609472632939346</v>
+        <v>0.031234939598316826</v>
       </c>
       <c r="B7" s="0">
-        <v>0.022455660357080794</v>
+        <v>0.013352422527120466</v>
       </c>
     </row>
     <row r="8" x14ac:dyDescent="0.3">
       <c r="A8" s="0">
-        <v>0.054613921415812297</v>
+        <v>0.031176549100875615</v>
       </c>
       <c r="B8" s="0">
-        <v>0.026927285554786826</v>
+        <v>0.015974278671041783</v>
       </c>
     </row>
     <row r="9" x14ac:dyDescent="0.3">
       <c r="A9" s="0">
-        <v>0.054210680841937725</v>
+        <v>0.030911785928368192</v>
       </c>
       <c r="B9" s="0">
-        <v>0.031576551645545008</v>
+        <v>0.018631053788633414</v>
       </c>
     </row>
     <row r="10" x14ac:dyDescent="0.3">
       <c r="A10" s="0">
-        <v>0.053371656443950879</v>
+        <v>0.03044297038281529</v>
       </c>
       <c r="B10" s="0">
-        <v>0.036363026633864759</v>
+        <v>0.021298681609308586</v>
       </c>
     </row>
     <row r="11" x14ac:dyDescent="0.3">
       <c r="A11" s="0">
-        <v>0.052082499189623141</v>
+        <v>0.029773757926402866</v>
       </c>
       <c r="B11" s="0">
-        <v>0.041230486985393291</v>
+        <v>0.023957023192411407</v>
       </c>
     </row>
     <row r="12" x14ac:dyDescent="0.3">
       <c r="A12" s="0">
-        <v>0.050357086187710884</v>
+        <v>0.028906578979824633</v>
       </c>
       <c r="B12" s="0">
-        <v>0.046100428261396431</v>
+        <v>0.026591095841910946</v>
       </c>
     </row>
     <row r="13" x14ac:dyDescent="0.3">
       <c r="A13" s="0">
-        <v>0.048223780792736072</v>
+        <v>0.02784029336220735</v>
       </c>
       <c r="B13" s="0">
-        <v>0.05090096160715616</v>
+        <v>0.029190915449779486</v>
       </c>
       <c r="D13">
         <f>(2*A13+A14)/3</f>
@@ -1657,34 +1657,34 @@
     </row>
     <row r="14" x14ac:dyDescent="0.3">
       <c r="A14" s="0">
-        <v>0.045716752002397665</v>
+        <v>0.026568387157913348</v>
       </c>
       <c r="B14" s="0">
-        <v>0.055575033055105603</v>
+        <v>0.031750288247939198</v>
       </c>
     </row>
     <row r="15" x14ac:dyDescent="0.3">
       <c r="A15" s="0">
-        <v>0.042871392895389909</v>
+        <v>0.02508232959574519</v>
       </c>
       <c r="B15" s="0">
-        <v>0.060080143518030246</v>
+        <v>0.034261625626509841</v>
       </c>
     </row>
     <row r="16" x14ac:dyDescent="0.3">
       <c r="A16" s="0">
-        <v>0.039725918830951598</v>
+        <v>0.023387971244823155</v>
       </c>
       <c r="B16" s="0">
-        <v>0.064383344765205061</v>
+        <v>0.036705054500755022</v>
       </c>
     </row>
     <row r="17" x14ac:dyDescent="0.3">
       <c r="A17" s="0">
-        <v>0.036315775911222495</v>
+        <v>0.021496069034282091</v>
       </c>
       <c r="B17" s="0">
-        <v>0.068462554299649953</v>
+        <v>0.039060298834845873</v>
       </c>
       <c r="D17">
         <f>(2*A17+A18)/3</f>
@@ -1713,74 +1713,74 @@
     </row>
     <row r="18" x14ac:dyDescent="0.3">
       <c r="A18" s="0">
-        <v>0.032668266040268561</v>
+        <v>0.01941781558147522</v>
       </c>
       <c r="B18" s="0">
-        <v>0.072305905715261853</v>
+        <v>0.041310044771103359</v>
       </c>
     </row>
     <row r="19" x14ac:dyDescent="0.3">
       <c r="A19" s="0">
-        <v>0.028807529528362463</v>
+        <v>0.017163718790668255</v>
       </c>
       <c r="B19" s="0">
-        <v>0.075905849649006013</v>
+        <v>0.043439789110732582</v>
       </c>
     </row>
     <row r="20" x14ac:dyDescent="0.3">
       <c r="A20" s="0">
-        <v>0.024752975572863989</v>
+        <v>0.014743255892444252</v>
       </c>
       <c r="B20" s="0">
-        <v>0.079258334607815728</v>
+        <v>0.045437163357475691</v>
       </c>
     </row>
     <row r="21" x14ac:dyDescent="0.3">
       <c r="A21" s="0">
-        <v>0.020518594965726871</v>
+        <v>0.012165412443227119</v>
       </c>
       <c r="B21" s="0">
-        <v>0.082361470216148119</v>
+        <v>0.047291085457566037</v>
       </c>
     </row>
     <row r="22" x14ac:dyDescent="0.3">
       <c r="A22" s="0">
-        <v>0.016112808446753661</v>
+        <v>0.0094401317148825915</v>
       </c>
       <c r="B22" s="0">
-        <v>0.085214098044140416</v>
+        <v>0.048991083679273455</v>
       </c>
     </row>
     <row r="23" x14ac:dyDescent="0.3">
       <c r="A23" s="0">
-        <v>0.011545958846154687</v>
+        <v>0.0065731265071155582</v>
       </c>
       <c r="B23" s="0">
-        <v>0.087813472752155883</v>
+        <v>0.050528095608198792</v>
       </c>
     </row>
     <row r="24" x14ac:dyDescent="0.3">
       <c r="A24" s="0">
-        <v>0.0068278173300964024</v>
+        <v>0.0035587101735440065</v>
       </c>
       <c r="B24" s="0">
-        <v>0.09015628435609771</v>
+        <v>0.051893504589564057</v>
       </c>
     </row>
     <row r="25" x14ac:dyDescent="0.3">
       <c r="A25" s="0">
-        <v>0.0019567796589698792</v>
+        <v>0.00038487777691255073</v>
       </c>
       <c r="B25" s="0">
-        <v>0.092238900267969187</v>
+        <v>0.05307552762253475</v>
       </c>
     </row>
     <row r="26" x14ac:dyDescent="0.3">
       <c r="A26" s="0">
-        <v>-0.0030804600690880327</v>
+        <v>-0.0029656632378995736</v>
       </c>
       <c r="B26" s="0">
-        <v>0.094054414893165517</v>
+        <v>0.054057172135719887</v>
       </c>
       <c r="D26">
         <f>(A26+2*A27)/3</f>
@@ -1809,34 +1809,34 @@
     </row>
     <row r="27" x14ac:dyDescent="0.3">
       <c r="A27" s="0">
-        <v>-0.0083086876604106189</v>
+        <v>-0.0065137780112569134</v>
       </c>
       <c r="B27" s="0">
-        <v>0.095589622163271257</v>
+        <v>0.054814329294629406</v>
       </c>
     </row>
     <row r="28" x14ac:dyDescent="0.3">
       <c r="A28" s="0">
-        <v>-0.013765667950279276</v>
+        <v>-0.010280391163594629</v>
       </c>
       <c r="B28" s="0">
-        <v>0.096821557401373978</v>
+        <v>0.055314322445300344</v>
       </c>
     </row>
     <row r="29" x14ac:dyDescent="0.3">
       <c r="A29" s="0">
-        <v>-0.019494133886322765</v>
+        <v>-0.014242098992306954</v>
       </c>
       <c r="B29" s="0">
-        <v>0.097714856836225925</v>
+        <v>0.055525649606486593</v>
       </c>
     </row>
     <row r="30" x14ac:dyDescent="0.3">
       <c r="A30" s="0">
-        <v>-0.025510566461094477</v>
+        <v>-0.018349660980057997</v>
       </c>
       <c r="B30" s="0">
-        <v>0.09822699164211747</v>
+        <v>0.055426106263442368</v>
       </c>
       <c r="D30">
         <f>(A30+2*A31)/3</f>
@@ -1865,82 +1865,242 @@
     </row>
     <row r="31" x14ac:dyDescent="0.3">
       <c r="A31" s="0">
-        <v>-0.031824224898798742</v>
+        <v>-0.022541691954509561</v>
       </c>
       <c r="B31" s="0">
-        <v>0.098308064056358863</v>
+        <v>0.055006520803706466</v>
       </c>
     </row>
     <row r="32" x14ac:dyDescent="0.3">
       <c r="A32" s="0">
-        <v>-0.038441814798410953</v>
+        <v>-0.026750911017145065</v>
       </c>
       <c r="B32" s="0">
-        <v>0.097899024303526774</v>
+        <v>0.054273101884406379</v>
       </c>
     </row>
     <row r="33" x14ac:dyDescent="0.3">
       <c r="A33" s="0">
-        <v>-0.045373789873514259</v>
+        <v>-0.030901619919662168</v>
       </c>
       <c r="B33" s="0">
-        <v>0.096926549962942657</v>
+        <v>0.053252793953515079</v>
       </c>
     </row>
     <row r="34" x14ac:dyDescent="0.3">
       <c r="A34" s="0">
-        <v>-0.052676077066566906</v>
+        <v>-0.034954033205832125</v>
       </c>
       <c r="B34" s="0">
-        <v>0.095273931826475838</v>
+        <v>0.051969498911221539</v>
       </c>
     </row>
     <row r="35" x14ac:dyDescent="0.3">
       <c r="A35" s="0">
-        <v>-0.060583471375479522</v>
+        <v>-0.038920636153665783</v>
       </c>
       <c r="B35" s="0">
-        <v>0.09266443728560031</v>
+        <v>0.050417200840244626</v>
       </c>
     </row>
     <row r="36" x14ac:dyDescent="0.3">
       <c r="A36" s="0">
-        <v>-0.06937696194366938</v>
+        <v>-0.042837807450057899</v>
       </c>
       <c r="B36" s="0">
-        <v>0.088633319515610001</v>
+        <v>0.048559065524243168</v>
       </c>
     </row>
     <row r="37" x14ac:dyDescent="0.3">
       <c r="A37" s="0">
-        <v>-0.078802608801258431</v>
+        <v>-0.046754051893864466</v>
       </c>
       <c r="B37" s="0">
-        <v>0.082933465702946935</v>
+        <v>0.046321954660580068</v>
       </c>
     </row>
     <row r="38" x14ac:dyDescent="0.3">
       <c r="A38" s="0">
-        <v>-0.088143875687268253</v>
+        <v>-0.050739121783802153</v>
       </c>
       <c r="B38" s="0">
-        <v>0.075789578780181596</v>
+        <v>0.043566780473718515</v>
       </c>
     </row>
     <row r="39" x14ac:dyDescent="0.3">
       <c r="A39" s="0">
-        <v>-0.096755831958152003</v>
+        <v>-0.054877922507997522</v>
       </c>
       <c r="B39" s="0">
-        <v>0.067706083296607336</v>
+        <v>0.040050570250862075</v>
       </c>
     </row>
     <row r="40" x14ac:dyDescent="0.3">
       <c r="A40" s="0">
-        <v>-0.10433335455158962</v>
+        <v>-0.059142549923437843</v>
       </c>
       <c r="B40" s="0">
-        <v>0.059157138171925819</v>
+        <v>0.035540945240013846</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0">
+        <v>-0.029330544062522997</v>
+      </c>
+      <c r="B41" s="0">
+        <v>0.047314086321386312</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0">
+        <v>-0.032529482723521859</v>
+      </c>
+      <c r="B42" s="0">
+        <v>0.046036423933391177</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0">
+        <v>-0.035700487754425136</v>
+      </c>
+      <c r="B43" s="0">
+        <v>0.044526346086814342</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0">
+        <v>-0.038826879500871027</v>
+      </c>
+      <c r="B44" s="0">
+        <v>0.042780594296847503</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0">
+        <v>-0.041893077029166143</v>
+      </c>
+      <c r="B45" s="0">
+        <v>0.040795173331206143</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0">
+        <v>-0.044888361294267327</v>
+      </c>
+      <c r="B46" s="0">
+        <v>0.038559902643114818</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0">
+        <v>-0.047801814062131499</v>
+      </c>
+      <c r="B47" s="0">
+        <v>0.036060468616549247</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0">
+        <v>-0.050627641032028874</v>
+      </c>
+      <c r="B48" s="0">
+        <v>0.033267661361455744</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0">
+        <v>-0.053346791264648759</v>
+      </c>
+      <c r="B49" s="0">
+        <v>0.030158323008008834</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0">
+        <v>-0.055914392174097043</v>
+      </c>
+      <c r="B50" s="0">
+        <v>0.026748445565299591</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0">
+        <v>-0.058267480416534186</v>
+      </c>
+      <c r="B51" s="0">
+        <v>0.023114456023117409</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="0">
+        <v>-0.060374419001357552</v>
+      </c>
+      <c r="B52" s="0">
+        <v>0.019307262676770937</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="0">
+        <v>-0.062228189217733688</v>
+      </c>
+      <c r="B53" s="0">
+        <v>0.01532780449043274</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="0">
+        <v>-0.063816171932330246</v>
+      </c>
+      <c r="B54" s="0">
+        <v>0.01119009996470678</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="0">
+        <v>-0.065124935683038704</v>
+      </c>
+      <c r="B55" s="0">
+        <v>0.0069197293738260694</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="0">
+        <v>-0.066144721707631096</v>
+      </c>
+      <c r="B56" s="0">
+        <v>0.0025334184544201989</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="0">
+        <v>-0.066864416563743229</v>
+      </c>
+      <c r="B57" s="0">
+        <v>-0.0020197733689228318</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="0">
+        <v>-0.067251466756522327</v>
+      </c>
+      <c r="B58" s="0">
+        <v>-0.0068221642828780911</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="0">
+        <v>-0.067249074379770735</v>
+      </c>
+      <c r="B59" s="0">
+        <v>-0.011925622520987033</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="0">
+        <v>-0.066807520966436773</v>
+      </c>
+      <c r="B60" s="0">
+        <v>-0.017255582931883569</v>
       </c>
     </row>
   </sheetData>

</xml_diff>